<commit_message>
feat: add web UI and fix Excel generation for timetables chore: ignore output_timetables directory
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_timetable.xlsx
+++ b/backend/output_timetables/sem1_timetable.xlsx
@@ -469,27 +469,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>MA101</t>
         </is>
       </c>
     </row>
@@ -501,12 +501,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -516,12 +516,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -565,27 +565,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>DS101</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>MA102</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
     </row>
@@ -602,22 +602,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS101</t>
         </is>
       </c>
     </row>
@@ -634,22 +634,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>EC101</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>HS101</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>MA101</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>EC101</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -707,12 +707,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -722,12 +722,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>MA101</t>
         </is>
       </c>
     </row>
@@ -744,22 +744,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -803,27 +803,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>DS101</t>
         </is>
       </c>
     </row>
@@ -835,27 +835,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>EC101</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>HS101</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>MA101</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151</t>
         </is>
       </c>
     </row>
@@ -867,7 +867,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">

</xml_diff>

<commit_message>
Added 2nd testcase and elective basket scheduling with common slots, enhanced visual coding
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_timetable.xlsx
+++ b/backend/output_timetables/sem1_timetable.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Section_A" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Section_B" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Course_Summary" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,12 +470,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -484,7 +485,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -501,12 +502,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -516,7 +517,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -565,27 +566,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>HS101</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
     </row>
@@ -597,27 +598,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>EC101</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>CS101</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>MA102</t>
         </is>
       </c>
     </row>
@@ -629,27 +630,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -707,27 +708,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -739,27 +740,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MA102</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>MA101</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>HS101</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CS101</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>MA102</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -803,27 +804,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
     </row>
@@ -835,17 +836,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -855,7 +856,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -867,27 +868,288 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>EC101</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Course Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>LTPSC</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Credits</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Instructor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MA101</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Dr. Ramesh Adve</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS101</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Introduction to DS and AI</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Dr. Abdul Wahid</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MA102</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Dr. Chintamani</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EC101</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3-0-0-2-5</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Dr. Prakash Pawar</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Problem Solving through Programming</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3-0-2-0-5</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Dr. Sunil P V</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HS101</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>English Language and Communication</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
+          <t>3-0-0-0-3</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>Dr. Rajesh N S</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Introduction to Cybersecurity</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Dr. Girish</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: resolve timetable regeneration issue with file uploads
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_timetable.xlsx
+++ b/backend/output_timetables/sem1_timetable.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC105</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,17 +480,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>CS105</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>MA105</t>
         </is>
       </c>
     </row>
@@ -507,22 +507,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS105</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>DS105</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS105</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA105</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>EC105</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>MA106</t>
         </is>
       </c>
     </row>
@@ -598,27 +598,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS105</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>HS105</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>CS155 (Elective)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>EC105</t>
         </is>
       </c>
     </row>
@@ -630,22 +630,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>HS105</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS105</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>MA106</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -708,27 +708,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>CS105</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS105</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA105</t>
         </is>
       </c>
     </row>
@@ -745,22 +745,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>MA105</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>CS105</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC105</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -809,22 +809,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>HS105</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>HS105</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>HS105</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>CS105</t>
         </is>
       </c>
     </row>
@@ -836,22 +836,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA106</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS105</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>CS155 (Elective)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -868,12 +868,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>EC105</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -883,12 +883,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>MA106</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>EC105</t>
         </is>
       </c>
     </row>
@@ -946,12 +946,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>MA105</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Statistical Methods</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -969,19 +969,19 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dr. Ramesh Adve</t>
+          <t>Dr. Priya Sharma</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>DS105</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Introduction to DS and AI</t>
+          <t>Fundamentals of Data Science</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -999,19 +999,19 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dr. Abdul Wahid</t>
+          <t>Dr. Rohan Verma</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>MA106</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Probability Theory</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1029,19 +1029,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dr. Chintamani</t>
+          <t>Dr. Sanjay Kumar</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>EC105</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>Digital Systems</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1059,19 +1059,19 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dr. Prakash Pawar</t>
+          <t>Dr. Anjali Mehta</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>CS105</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Problem Solving through Programming</t>
+          <t>Programming Fundamentals</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1089,19 +1089,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Dr. Sunil P V</t>
+          <t>Dr. Vikram Joshi</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>HS105</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>English Language and Communication</t>
+          <t>Professional Communication</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1119,19 +1119,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dr. Rajesh N S</t>
+          <t>Dr. Rajeev Malhotra</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>CS155</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Introduction to Cybersecurity</t>
+          <t>Cybersecurity Basics</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Dr. Girish</t>
+          <t>Dr. Kavya Iyer</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: ensure elective courses are scheduled in same time slots for both sections A and B
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_timetable.xlsx
+++ b/backend/output_timetables/sem1_timetable.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Section_A" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Section_B" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Course_Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Elective_Coordination" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -470,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>EC105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,17 +481,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CS105</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MA105</t>
+          <t>MA101</t>
         </is>
       </c>
     </row>
@@ -502,27 +503,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>HS105</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DS105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CS105</t>
+          <t>DS101</t>
         </is>
       </c>
     </row>
@@ -566,12 +567,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MA105</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EC105</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -581,12 +582,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MA106</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -598,27 +599,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CS105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>HS105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS155 (Elective)</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>EC105</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
     </row>
@@ -630,17 +631,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>HS105</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DS105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>MA106</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -650,7 +651,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
     </row>
@@ -708,12 +709,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CS105</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -723,12 +724,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DS105</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MA105</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -745,22 +746,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MA105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CS105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EC105</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
     </row>
@@ -804,27 +805,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HS105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>HS105</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>HS105</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS105</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -836,27 +837,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MA106</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>DS105</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS155 (Elective)</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA102</t>
         </is>
       </c>
     </row>
@@ -868,27 +869,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>EC105</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>MA106</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EC105</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -946,12 +947,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MA105</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Statistical Methods</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -969,19 +970,19 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dr. Priya Sharma</t>
+          <t>Dr. Ramesh Adve</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DS105</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fundamentals of Data Science</t>
+          <t>Introduction to DS and AI</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -999,19 +1000,19 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dr. Rohan Verma</t>
+          <t>Dr. Abdul Wahid</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MA106</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Probability Theory</t>
+          <t>Probability</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1029,19 +1030,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dr. Sanjay Kumar</t>
+          <t>Dr. Chintamani</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EC105</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Digital Systems</t>
+          <t>Digital Design</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1059,19 +1060,19 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dr. Anjali Mehta</t>
+          <t>Dr. Prakash Pawar</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CS105</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Programming Fundamentals</t>
+          <t>Problem Solving through Programming</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1089,19 +1090,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Dr. Vikram Joshi</t>
+          <t>Dr. Sunil P V</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HS105</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Professional Communication</t>
+          <t>English Language and Communication</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1119,19 +1120,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dr. Rajeev Malhotra</t>
+          <t>Dr. Rajesh N S</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CS155</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cybersecurity Basics</t>
+          <t>Introduction to Cybersecurity</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1149,7 +1150,80 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Dr. Kavya Iyer</t>
+          <t>Dr. Girish</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Elective Course</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Time Slot</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Slot Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Sections</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>15:30-17:00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Elective_Slot_1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>A &amp; B (Common Slot)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix elective course scheduling to use common time slots for both sections
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_timetable.xlsx
+++ b/backend/output_timetables/sem1_timetable.xlsx
@@ -481,12 +481,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -503,12 +503,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -567,22 +567,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>HS101</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>HS101</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>EC101</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>DS101</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -609,17 +609,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>DS101</t>
         </is>
       </c>
     </row>
@@ -631,22 +631,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -709,27 +709,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>HS101</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>DS101</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -756,12 +756,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>HS101</t>
         </is>
       </c>
     </row>
@@ -805,7 +805,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -815,17 +815,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -837,22 +837,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -874,17 +874,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">

</xml_diff>

<commit_message>
Changed duration of tutorials to 1hr
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_timetable.xlsx
+++ b/backend/output_timetables/sem1_timetable.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,27 +471,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -513,12 +513,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -567,19 +567,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MA102</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>HS101</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>HS101</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>EC101</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>Free</t>
@@ -587,7 +587,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -599,12 +599,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -631,27 +631,187 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>HS101</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>MA102</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>EC101</t>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>15:30-16:30</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>16:30-17:30</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>17:30-18:30</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -666,7 +826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -714,7 +874,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -729,7 +889,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>MA102</t>
         </is>
       </c>
     </row>
@@ -741,27 +901,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>EC101</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>MA101</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>HS101</t>
         </is>
       </c>
     </row>
@@ -805,12 +965,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -820,12 +980,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -837,27 +997,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>MA101</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>HS101</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>CS151 (Elective)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>DS101</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CS101</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>CS151 (Elective)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>MA102</t>
         </is>
       </c>
     </row>
@@ -869,25 +1029,185 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
+        <is>
+          <t>HS101</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>13:00-14:00</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>15:30-16:30</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>16:30-17:30</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>17:30-18:30</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
@@ -904,7 +1224,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -935,10 +1255,20 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Credits</t>
+          <t>Lectures/Week</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Tutorials/Week</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total Credits</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Instructor</t>
         </is>
@@ -968,9 +1298,15 @@
       <c r="E2" t="n">
         <v>2</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Dr. Ramesh Adve</t>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Dr. Meera Nair</t>
         </is>
       </c>
     </row>
@@ -998,9 +1334,15 @@
       <c r="E3" t="n">
         <v>2</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Dr. Abdul Wahid</t>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Dr. Arjun Deshmukh</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1370,13 @@
       <c r="E4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Dr. Chintamani</t>
         </is>
@@ -1056,11 +1404,17 @@
         </is>
       </c>
       <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
         <v>5</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Dr. Prakash Pawar</t>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Dr. Kavita Bansal</t>
         </is>
       </c>
     </row>
@@ -1086,11 +1440,17 @@
         </is>
       </c>
       <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
         <v>5</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Dr. Sunil P V</t>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Dr. Suresh Kulkarni</t>
         </is>
       </c>
     </row>
@@ -1118,7 +1478,13 @@
       <c r="E7" t="n">
         <v>3</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>Dr. Rajesh N S</t>
         </is>
@@ -1148,9 +1514,15 @@
       <c r="E8" t="n">
         <v>2</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Dr. Girish</t>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Dr. Neel Patel</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: enhance timetable with structured LTPSC compliance and unified time slot styling
- Apply consistent color coding: blue for 1.5h lectures, green for 1h tutorials, orange for lunch
- Strictly enforce LTPSC structure ensuring accurate session counts and types
- Optimize chronological flow with proper session sequencing
- Improve visual hierarchy and user interaction
- Improve Settings section
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_timetable.xlsx
+++ b/backend/output_timetables/sem1_timetable.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,32 +466,32 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>9:00-10:30</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MA102</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>MA102</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>HS101</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>EC101</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>EC101</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CS101</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>EC101</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -508,29 +508,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>12:30-14:00</t>
+          <t>12:00-13:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -562,49 +562,49 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>14:00-15:30</t>
+          <t>13:00-14:30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>MA101</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>HS101</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>15:30-17:00</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -626,39 +626,39 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>17:00-18:30</t>
+          <t>15:30-17:00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>CS101</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>MA101</t>
-        </is>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>DS101</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>12:00-13:00</t>
+          <t>17:00-18:00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Tutorial)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -682,134 +682,6 @@
         </is>
       </c>
       <c r="F8" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>15:30-16:30</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>16:30-17:30</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>17:30-18:30</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
@@ -826,7 +698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -864,32 +736,32 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>9:00-10:30</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>EC101</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>CS101</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>DS101</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>CS101</t>
         </is>
       </c>
     </row>
@@ -911,24 +783,24 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS101</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA101</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>12:30-14:00</t>
+          <t>12:00-13:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -960,103 +832,103 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>14:00-15:30</t>
+          <t>13:00-14:30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA102</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>EC101</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>MA101</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>15:30-17:00</t>
+          <t>14:30-15:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MA102</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MA101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DS101</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>17:00-18:30</t>
+          <t>15:30-17:00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>EC101</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>HS101</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>HS101</t>
+          <t>MA102</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>12:00-13:00</t>
+          <t>17:00-18:00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1066,7 +938,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Tutorial)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1080,134 +952,6 @@
         </is>
       </c>
       <c r="F8" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>13:00-14:00</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>15:30-16:30</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>16:30-17:30</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>17:30-18:30</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
@@ -1306,7 +1050,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Dr. Meera Nair</t>
+          <t>Dr. Ramesh Adve</t>
         </is>
       </c>
     </row>
@@ -1342,7 +1086,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Dr. Arjun Deshmukh</t>
+          <t>Dr. Abdul Wahid</t>
         </is>
       </c>
     </row>
@@ -1414,7 +1158,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dr. Kavita Bansal</t>
+          <t>Dr. Prakash Pawar</t>
         </is>
       </c>
     </row>
@@ -1450,7 +1194,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Dr. Suresh Kulkarni</t>
+          <t>Dr. Sunil P V</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1266,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Dr. Neel Patel</t>
+          <t>Dr. Girish</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1553,20 +1297,25 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Session Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Day</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Time Slot</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Slot Name</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Sections</t>
         </is>
@@ -1580,20 +1329,89 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Lecture 1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10:30-12:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1.5 hours</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>A &amp; B (Common Slot)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Lecture 2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Thu</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>15:30-17:00</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Elective_Slot_1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1.5 hours</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>A &amp; B (Common Slot)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tutorial</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1 hour</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>A &amp; B (Common Slot)</t>
         </is>

</xml_diff>